<commit_message>
Background Research - Introduction to Quantum Computing
</commit_message>
<xml_diff>
--- a/Documentation/References.xlsx
+++ b/Documentation/References.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GDrive\MSc\Dissertation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GDrive\MSc\Dissertation\git\QuantumExperiments\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD87D4FD-C6C0-4518-BE6C-C4065C5838F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC83B3E-BE33-470B-B4AA-897AC3C08F46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A41E5D1C-7FC4-4D22-A116-A8D00D3FF93A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>https://cloudblogs.microsoft.com/quantum</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Andy Matuschak and Michael A. Nielsen, “Quantum Computing for the Very Curious”, https://quantum.country/qcvc, San Francisco (2019).</t>
+  </si>
+  <si>
+    <t>Circuit-centric quantum classifiers</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1804.00633.pdf</t>
+  </si>
+  <si>
+    <t>Maria Schuld, Alex Bocharov, Krysta Svore, and Nathan Wiebe</t>
   </si>
 </sst>
 </file>
@@ -486,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D39EB2C-760E-4F64-8B15-BF3554152337}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,6 +608,17 @@
       </c>
       <c r="B12" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -615,8 +635,9 @@
     <hyperlink ref="A10" r:id="rId10" xr:uid="{4B11EEC8-18A7-4308-BE94-0FCF81F07774}"/>
     <hyperlink ref="A11" r:id="rId11" xr:uid="{8795E619-54F2-4FC8-B016-2B76AB765BA9}"/>
     <hyperlink ref="A12" r:id="rId12" xr:uid="{13499EC8-2E43-42AA-BB76-1C013CE02E22}"/>
+    <hyperlink ref="A13" r:id="rId13" xr:uid="{2D7CF04C-F997-4487-BE8E-CE10CD251CE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Background Research on Quantum Algorithms
</commit_message>
<xml_diff>
--- a/Documentation/References.xlsx
+++ b/Documentation/References.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GDrive\MSc\Dissertation\git\QuantumExperiments\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC83B3E-BE33-470B-B4AA-897AC3C08F46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CCC754-AA7C-4C32-B4E0-118BB8868066}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A41E5D1C-7FC4-4D22-A116-A8D00D3FF93A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>https://cloudblogs.microsoft.com/quantum</t>
   </si>
@@ -118,6 +118,33 @@
   </si>
   <si>
     <t>Maria Schuld, Alex Bocharov, Krysta Svore, and Nathan Wiebe</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9Iorl3MUF-Y</t>
+  </si>
+  <si>
+    <t>Grovers Algorithm, Best explanation by Umesh Vazirani</t>
+  </si>
+  <si>
+    <t>Qiskit Textbook</t>
+  </si>
+  <si>
+    <t>Qiskit-Textbook,
+       author = {Abraham Asfaw, Luciano Bello, Yael Ben-Haim, Sergey Bravyi, Nicholas Bronn, Lauren Capelluto, Almudena Carrera Vazquez, Jack Ceroni,  Richard Chen, Albert Frisch, Jay Gambetta, Shelly Garion, Leron Gil, Salvador De La Puente Gonzalez, Francis Harkins, Takashi Imamichi, David McKay, Antonio Mezzacapo, Zlatko Minev, Ramis Movassagh, Giacomo Nannicni, Paul Nation,  Anna Phan, Marco Pistoia, Arthur Rattew, Joachim Schaefer, Javad Shabani, John Smolin, Kristan Temme, Madeleine Tod, Stephen Wood, James Wootton.},
+       title = {Learn Quantum Computation Using Qiskit},
+       year = {2020},
+       url = {http://community.qiskit.org/textbook},
+@misc{ Qiskit-Textbook,
+       author = {Abraham Asfaw, Luciano Bello, Yael Ben-Haim, Sergey Bravyi, Nicholas Bronn, Lauren Capelluto, Almudena Carrera Vazquez, Jack Ceroni,  Richard Chen, Albert Frisch, Jay Gambetta, Shelly Garion, Leron Gil, Salvador De La Puente Gonzalez, Francis Harkins, Takashi Imamichi, David McKay, Antonio Mezzacapo, Zlatko Minev, Ramis Movassagh, Giacomo Nannicni, Paul Nation,  Anna Phan, Marco Pistoia, Arthur Rattew, Joachim Schaefer, Javad Shabani, John Smolin, Kristan Temme, Madeleine Tod, Stephen Wood, James Wootton.},
+       title = {Learn Quantum Computation Using Qiskit},
+       year = {2020},
+       url = {http://community.qiskit.org/textbook},
+@misc{ Qiskit-Textbook,
+       author = {Abraham Asfaw, Luciano Bello, Yael Ben-Haim, Sergey Bravyi, Nicholas Bronn, Lauren Capelluto, Almudena Carrera Vazquez, Jack Ceroni,  Richard Chen, Albert Frisch, Jay Gambetta, Shelly Garion, Leron Gil, Salvador De La Puente Gonzalez, Francis Harkins, Takashi Imamichi, David McKay, Antonio Mezzacapo, Zlatko Minev, Ramis Movassagh, Giacomo Nannicni, Paul Nation,  Anna Phan, Marco Pistoia, Arthur Rattew, Joachim Schaefer, Javad Shabani, John Smolin, Kristan Temme, Madeleine Tod, Stephen Wood, James Wootton.},
+       title = {Learn Quantum Computation Using Qiskit},
+       year = {2020},
+       url = {http://community.qiskit.org/textbook},
+}</t>
   </si>
 </sst>
 </file>
@@ -495,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D39EB2C-760E-4F64-8B15-BF3554152337}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,6 +646,22 @@
       </c>
       <c r="C13" s="3" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -636,8 +679,9 @@
     <hyperlink ref="A11" r:id="rId11" xr:uid="{8795E619-54F2-4FC8-B016-2B76AB765BA9}"/>
     <hyperlink ref="A12" r:id="rId12" xr:uid="{13499EC8-2E43-42AA-BB76-1C013CE02E22}"/>
     <hyperlink ref="A13" r:id="rId13" xr:uid="{2D7CF04C-F997-4487-BE8E-CE10CD251CE5}"/>
+    <hyperlink ref="A14" r:id="rId14" xr:uid="{5F2F95F1-03A8-45CD-9C46-BB8C421F5682}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Accuracy of 55% with one CyclicEntanglingLayer, 2. Added Classical SVM classifier, 3. Dissertation Presentation
</commit_message>
<xml_diff>
--- a/Documentation/References.xlsx
+++ b/Documentation/References.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GDrive\MSc\Dissertation\git\QuantumExperiments\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CCC754-AA7C-4C32-B4E0-118BB8868066}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD46C65-4F30-4C40-AF89-2909ECF37E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A41E5D1C-7FC4-4D22-A116-A8D00D3FF93A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>https://cloudblogs.microsoft.com/quantum</t>
   </si>
@@ -145,6 +145,9 @@
        year = {2020},
        url = {http://community.qiskit.org/textbook},
 }</t>
+  </si>
+  <si>
+    <t>Channel: 3Blue1Brown</t>
   </si>
 </sst>
 </file>
@@ -524,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D39EB2C-760E-4F64-8B15-BF3554152337}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,6 +638,9 @@
       </c>
       <c r="B12" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>